<commit_message>
Listo el análisis, sería bueno encontrar graficos para agregar a las diapositivas para explicar los algoritmos.
</commit_message>
<xml_diff>
--- a/Problema-Mochila/Resultados/plantilla_resultados.xlsx
+++ b/Problema-Mochila/Resultados/plantilla_resultados.xlsx
@@ -415,6 +415,12 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -439,12 +445,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -749,43 +749,43 @@
   <dimension ref="C3:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.75" customWidth="1"/>
-    <col min="4" max="6" width="11.625" customWidth="1"/>
-    <col min="7" max="7" width="11.375" customWidth="1"/>
-    <col min="8" max="15" width="11.625" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="8" max="15" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:15" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="10"/>
-      <c r="D4" s="12" t="s">
+      <c r="C4" s="16"/>
+      <c r="D4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="12" t="s">
+      <c r="E4" s="19"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="12" t="s">
+      <c r="H4" s="19"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="K4" s="13"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="15" t="s">
+      <c r="K4" s="19"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="16"/>
-      <c r="O4" s="17"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="23"/>
     </row>
     <row r="5" spans="3:15" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="11"/>
+      <c r="C5" s="17"/>
       <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
@@ -831,16 +831,16 @@
         <v>0.11122233300000001</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="F6" s="18"/>
+      <c r="F6" s="10"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="18"/>
+      <c r="I6" s="10"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
-      <c r="L6" s="18"/>
+      <c r="L6" s="10"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
-      <c r="O6" s="21"/>
+      <c r="O6" s="13"/>
     </row>
     <row r="7" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
@@ -848,16 +848,16 @@
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="7"/>
-      <c r="F7" s="19"/>
+      <c r="F7" s="11"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
-      <c r="I7" s="19"/>
+      <c r="I7" s="11"/>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
-      <c r="L7" s="19"/>
+      <c r="L7" s="11"/>
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
-      <c r="O7" s="22"/>
+      <c r="O7" s="14"/>
     </row>
     <row r="8" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="2" t="s">
@@ -865,16 +865,16 @@
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="7"/>
-      <c r="F8" s="19"/>
+      <c r="F8" s="11"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="19"/>
+      <c r="I8" s="11"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
-      <c r="L8" s="19"/>
+      <c r="L8" s="11"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
-      <c r="O8" s="22"/>
+      <c r="O8" s="14"/>
     </row>
     <row r="9" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
@@ -882,16 +882,16 @@
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="7"/>
-      <c r="F9" s="19"/>
+      <c r="F9" s="11"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="19"/>
+      <c r="I9" s="11"/>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
-      <c r="L9" s="19"/>
+      <c r="L9" s="11"/>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
-      <c r="O9" s="22"/>
+      <c r="O9" s="14"/>
     </row>
     <row r="10" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
@@ -899,16 +899,16 @@
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="7"/>
-      <c r="F10" s="19"/>
+      <c r="F10" s="11"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
-      <c r="I10" s="19"/>
+      <c r="I10" s="11"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
-      <c r="L10" s="19"/>
+      <c r="L10" s="11"/>
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
-      <c r="O10" s="22"/>
+      <c r="O10" s="14"/>
     </row>
     <row r="11" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="2" t="s">
@@ -916,16 +916,16 @@
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="7"/>
-      <c r="F11" s="19"/>
+      <c r="F11" s="11"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
-      <c r="I11" s="19"/>
+      <c r="I11" s="11"/>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
-      <c r="L11" s="19"/>
+      <c r="L11" s="11"/>
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
-      <c r="O11" s="22"/>
+      <c r="O11" s="14"/>
     </row>
     <row r="12" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="2" t="s">
@@ -933,16 +933,16 @@
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="7"/>
-      <c r="F12" s="19"/>
+      <c r="F12" s="11"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
-      <c r="I12" s="19"/>
+      <c r="I12" s="11"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
-      <c r="L12" s="19"/>
+      <c r="L12" s="11"/>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
-      <c r="O12" s="22"/>
+      <c r="O12" s="14"/>
     </row>
     <row r="13" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
@@ -950,16 +950,16 @@
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="7"/>
-      <c r="F13" s="19"/>
+      <c r="F13" s="11"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
-      <c r="I13" s="19"/>
+      <c r="I13" s="11"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
-      <c r="L13" s="19"/>
+      <c r="L13" s="11"/>
       <c r="M13" s="7"/>
       <c r="N13" s="7"/>
-      <c r="O13" s="22"/>
+      <c r="O13" s="14"/>
     </row>
     <row r="14" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="2" t="s">
@@ -967,16 +967,16 @@
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="7"/>
-      <c r="F14" s="19"/>
+      <c r="F14" s="11"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
-      <c r="I14" s="19"/>
+      <c r="I14" s="11"/>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
-      <c r="L14" s="19"/>
+      <c r="L14" s="11"/>
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
-      <c r="O14" s="22"/>
+      <c r="O14" s="14"/>
     </row>
     <row r="15" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="2" t="s">
@@ -984,16 +984,16 @@
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="7"/>
-      <c r="F15" s="19"/>
+      <c r="F15" s="11"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
-      <c r="I15" s="19"/>
+      <c r="I15" s="11"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
-      <c r="L15" s="19"/>
+      <c r="L15" s="11"/>
       <c r="M15" s="7"/>
       <c r="N15" s="7"/>
-      <c r="O15" s="22"/>
+      <c r="O15" s="14"/>
     </row>
     <row r="16" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="2" t="s">
@@ -1001,16 +1001,16 @@
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="7"/>
-      <c r="F16" s="19"/>
+      <c r="F16" s="11"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
-      <c r="I16" s="19"/>
+      <c r="I16" s="11"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
-      <c r="L16" s="19"/>
+      <c r="L16" s="11"/>
       <c r="M16" s="7"/>
       <c r="N16" s="7"/>
-      <c r="O16" s="22"/>
+      <c r="O16" s="14"/>
     </row>
     <row r="17" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="2" t="s">
@@ -1018,16 +1018,16 @@
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="7"/>
-      <c r="F17" s="19"/>
+      <c r="F17" s="11"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
-      <c r="I17" s="19"/>
+      <c r="I17" s="11"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
-      <c r="L17" s="19"/>
+      <c r="L17" s="11"/>
       <c r="M17" s="7"/>
       <c r="N17" s="7"/>
-      <c r="O17" s="22"/>
+      <c r="O17" s="14"/>
     </row>
     <row r="18" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="2" t="s">
@@ -1035,16 +1035,16 @@
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="7"/>
-      <c r="F18" s="19"/>
+      <c r="F18" s="11"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
-      <c r="I18" s="19"/>
+      <c r="I18" s="11"/>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
-      <c r="L18" s="19"/>
+      <c r="L18" s="11"/>
       <c r="M18" s="7"/>
       <c r="N18" s="7"/>
-      <c r="O18" s="22"/>
+      <c r="O18" s="14"/>
     </row>
     <row r="19" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C19" s="2" t="s">
@@ -1052,16 +1052,16 @@
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="7"/>
-      <c r="F19" s="19"/>
+      <c r="F19" s="11"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
-      <c r="I19" s="19"/>
+      <c r="I19" s="11"/>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
-      <c r="L19" s="19"/>
+      <c r="L19" s="11"/>
       <c r="M19" s="7"/>
       <c r="N19" s="7"/>
-      <c r="O19" s="22"/>
+      <c r="O19" s="14"/>
     </row>
     <row r="20" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="2" t="s">
@@ -1069,16 +1069,16 @@
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="9"/>
-      <c r="F20" s="20"/>
+      <c r="F20" s="12"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
-      <c r="I20" s="20"/>
+      <c r="I20" s="12"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
-      <c r="L20" s="20"/>
+      <c r="L20" s="12"/>
       <c r="M20" s="9"/>
       <c r="N20" s="9"/>
-      <c r="O20" s="23"/>
+      <c r="O20" s="15"/>
     </row>
     <row r="21" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="2" t="s">
@@ -1086,67 +1086,67 @@
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="9"/>
-      <c r="F21" s="20"/>
+      <c r="F21" s="12"/>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
-      <c r="I21" s="20"/>
+      <c r="I21" s="12"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
-      <c r="L21" s="20"/>
+      <c r="L21" s="12"/>
       <c r="M21" s="9"/>
       <c r="N21" s="9"/>
-      <c r="O21" s="23"/>
+      <c r="O21" s="15"/>
     </row>
     <row r="22" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D22" s="3">
-        <f t="shared" ref="D22:L22" si="0">SUM(D6:D21)/16</f>
-        <v>6.9513958125000004E-3</v>
+        <f>SUM(D6:D18)/13</f>
+        <v>8.5555640769230772E-3</v>
       </c>
       <c r="E22" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(E6:E18)/13</f>
         <v>0</v>
       </c>
       <c r="F22" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(F6:F18)/13</f>
         <v>0</v>
       </c>
       <c r="G22" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(G6:G18)/13</f>
         <v>0</v>
       </c>
       <c r="H22" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(H6:H18)/13</f>
         <v>0</v>
       </c>
       <c r="I22" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(I6:I18)/13</f>
         <v>0</v>
       </c>
       <c r="J22" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(J6:J18)/13</f>
         <v>0</v>
       </c>
       <c r="K22" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(K6:K18)/13</f>
         <v>0</v>
       </c>
       <c r="L22" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(L6:L18)/13</f>
         <v>0</v>
       </c>
       <c r="M22" s="3">
-        <f t="shared" ref="M22:O22" si="1">SUM(M6:M21)/16</f>
+        <f>SUM(M6:M18)/13</f>
         <v>0</v>
       </c>
       <c r="N22" s="3">
-        <f t="shared" si="1"/>
+        <f>SUM(N6:N18)/13</f>
         <v>0</v>
       </c>
       <c r="O22" s="3">
-        <f t="shared" si="1"/>
+        <f>SUM(O6:O18)/13</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>